<commit_message>
chore: add MkDocs/RTD docs + adapter cleanup + paper repro updates
</commit_message>
<xml_diff>
--- a/paper/journal_source_data/SourceData_EDFig3.xlsx
+++ b/paper/journal_source_data/SourceData_EDFig3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kfurudate/dev/LLM-PathwayCurator/paper/journal_source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9776E5-C9FF-3D40-82FA-ED51640B36CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1379709-89AA-4646-B86C-8231515AF529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6740" yWindow="1380" windowWidth="23500" windowHeight="12840" xr2:uid="{30EB6BB9-ED82-374A-B580-C38CF118DFA7}"/>
   </bookViews>
@@ -296,16 +296,16 @@
     <t>・llm (ours) = Proposed (matched context; LLM-assisted)</t>
   </si>
   <si>
-    <t>EDFig2a_pass_vs_human_risk</t>
-  </si>
-  <si>
-    <t>EDFig2b_abstain_reasons</t>
-  </si>
-  <si>
     <t>・EDFig3b_abstain_reasons: ABSTAIN reason-code composition (HNSC; LLM-assisted setting under Proposed at tau=0.8; panel b).</t>
   </si>
   <si>
     <t>・EDFig3a_pass_vs_human_risk: PASS rate vs human non-accept risk (HNSC; LLM-assisted setting under Proposed at tau=0.8; panel a).</t>
+  </si>
+  <si>
+    <t>EDFig3b_abstain_reasons</t>
+  </si>
+  <si>
+    <t>EDFig3a_pass_vs_human_risk</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
   <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C47" sqref="C1:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,12 +736,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -832,7 +832,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
@@ -872,7 +872,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>